<commit_message>
Revise "The Great Escape" document to enhance narrative and character roles
</commit_message>
<xml_diff>
--- a/public/data/_work-in-progress/_share/schedule.xlsx
+++ b/public/data/_work-in-progress/_share/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkland\Documents\projects-personal\scribbles\public\data\_work-in-progress\_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E892896-61A4-4DD8-8C03-68DAAD27DE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB30805-57E6-46D5-9DC7-8E6075847692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +636,7 @@
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>45660</v>
       </c>
@@ -660,7 +660,7 @@
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <f t="shared" si="0"/>
         <v>45674</v>
       </c>
@@ -672,7 +672,7 @@
       <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <f t="shared" si="0"/>
         <v>45681</v>
       </c>

</xml_diff>

<commit_message>
Cover images, schedule, etc. (Share)
</commit_message>
<xml_diff>
--- a/public/data/_work-in-progress/_share/schedule.xlsx
+++ b/public/data/_work-in-progress/_share/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkland\Documents\projects-personal\scribbles\public\data\_work-in-progress\_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB30805-57E6-46D5-9DC7-8E6075847692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5214471B-B55E-4D29-A0A4-94E26EE1B78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -514,7 +515,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +649,7 @@
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>45667</v>
       </c>
@@ -660,7 +661,7 @@
       <c r="B12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="5">
         <f t="shared" si="0"/>
         <v>45674</v>
       </c>
@@ -684,7 +685,7 @@
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <f t="shared" si="0"/>
         <v>45688</v>
       </c>
@@ -696,7 +697,7 @@
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <f t="shared" si="0"/>
         <v>45695</v>
       </c>
@@ -708,7 +709,7 @@
       <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <f t="shared" si="0"/>
         <v>45702</v>
       </c>
@@ -720,7 +721,7 @@
       <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <f t="shared" si="0"/>
         <v>45709</v>
       </c>

</xml_diff>

<commit_message>
Update more export imgs
</commit_message>
<xml_diff>
--- a/public/data/_work-in-progress/_share/schedule.xlsx
+++ b/public/data/_work-in-progress/_share/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkland\Documents\projects-personal\scribbles\public\data\_work-in-progress\_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AAA53A-1A29-4017-95EE-725AD4BDB2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3D6B7-B638-4980-B7A5-C4B34D3BCEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +732,7 @@
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>45716</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>45723</v>
       </c>
@@ -756,7 +756,7 @@
       <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="5">
         <f t="shared" si="0"/>
         <v>45730</v>
       </c>
@@ -780,7 +780,7 @@
       <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <f t="shared" si="0"/>
         <v>45744</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <f t="shared" si="0"/>
         <v>45751</v>
       </c>

</xml_diff>

<commit_message>
Add initial notes and update schedule and cover images in work-in-progress
</commit_message>
<xml_diff>
--- a/public/data/_work-in-progress/_share/schedule.xlsx
+++ b/public/data/_work-in-progress/_share/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkland\Documents\projects-personal\scribbles\public\data\_work-in-progress\_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF3D6B7-B638-4980-B7A5-C4B34D3BCEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6442B78-C0DB-4DEF-864A-45725478B397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="2610" windowWidth="12150" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -105,30 +105,18 @@
     <t>Something Borrowed, Something Blue</t>
   </si>
   <si>
-    <t>M: Law &amp; Trade</t>
-  </si>
-  <si>
     <t>Heavy Medal</t>
   </si>
   <si>
-    <t>M: Military &amp; Nobility</t>
-  </si>
-  <si>
     <t>Smuggler's Slip</t>
   </si>
   <si>
-    <t>M: Underworld &amp; Strange</t>
-  </si>
-  <si>
     <t>Water Under the Bridge</t>
   </si>
   <si>
     <t>A Murder of Crows</t>
   </si>
   <si>
-    <t>M: Academia &amp; Labor</t>
-  </si>
-  <si>
     <t>The Haunting of Hyle Hall</t>
   </si>
   <si>
@@ -139,6 +127,9 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Electric Dreams</t>
   </si>
 </sst>
 </file>
@@ -513,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5">
         <v>45614</v>
@@ -552,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" s="5">
         <v>45614</v>
@@ -563,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="5">
         <v>45618</v>
@@ -574,7 +565,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" s="5">
         <f>C4 + 7</f>
@@ -586,7 +577,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" ref="C6:C32" si="0">C5 + 7</f>
@@ -598,7 +589,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
@@ -610,7 +601,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5">
         <f t="shared" si="0"/>
@@ -622,7 +613,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5">
         <f t="shared" si="0"/>
@@ -634,7 +625,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5">
         <f t="shared" si="0"/>
@@ -646,7 +637,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" s="5">
         <f t="shared" si="0"/>
@@ -658,7 +649,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C12" s="5">
         <f t="shared" si="0"/>
@@ -670,7 +661,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5">
         <f t="shared" si="0"/>
@@ -682,7 +673,7 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5">
         <f t="shared" si="0"/>
@@ -694,7 +685,7 @@
         <v>16</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5">
         <f t="shared" si="0"/>
@@ -706,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5">
         <f t="shared" si="0"/>
@@ -718,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5">
         <f t="shared" si="0"/>
@@ -730,7 +721,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5">
         <f t="shared" si="0"/>
@@ -742,7 +733,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5">
         <f t="shared" si="0"/>
@@ -754,7 +745,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5">
         <f t="shared" si="0"/>
@@ -766,19 +757,19 @@
         <v>22</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="3">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5">
         <f t="shared" si="0"/>
         <v>45737</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3">
         <f t="shared" si="0"/>
@@ -787,10 +778,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" si="0"/>
@@ -799,22 +790,22 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="0"/>
+        <f>C23 + 7</f>
         <v>45758</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" si="0"/>
@@ -823,22 +814,22 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C26" s="4">
-        <f t="shared" si="0"/>
+        <f>C25 + 7</f>
         <v>45772</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="0"/>
@@ -847,10 +838,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="0"/>
@@ -859,10 +850,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="0"/>
@@ -870,11 +861,8 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="0"/>
@@ -882,11 +870,8 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="0"/>
@@ -894,11 +879,8 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C32" s="4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Refactor App.vue layout, update styles, and add Scoundry info component
</commit_message>
<xml_diff>
--- a/public/data/_work-in-progress/_share/schedule.xlsx
+++ b/public/data/_work-in-progress/_share/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirkland\Documents\projects-personal\scribbles\public\data\_work-in-progress\_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6442B78-C0DB-4DEF-864A-45725478B397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC850ED9-C61F-422B-8AB3-931D4A651DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2610" windowWidth="12150" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +771,7 @@
       <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="5">
         <f t="shared" si="0"/>
         <v>45744</v>
       </c>
@@ -783,7 +783,7 @@
       <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="5">
         <f t="shared" si="0"/>
         <v>45751</v>
       </c>
@@ -795,7 +795,7 @@
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <f>C23 + 7</f>
         <v>45758</v>
       </c>
@@ -807,7 +807,7 @@
       <c r="B25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f t="shared" si="0"/>
         <v>45765</v>
       </c>

</xml_diff>